<commit_message>
1 NF 2NF dan 3NF
</commit_message>
<xml_diff>
--- a/Sistem_Informasi_Penjualan.xlsx
+++ b/Sistem_Informasi_Penjualan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATERI SEMESTER 5\Studi Independen\PPT MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ED81D1-8B67-4341-8A95-DA8F47388B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5478F033-5C6C-4DC9-9B2D-80F30A253247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AAC0253C-ABCB-43A3-8073-8AEC6CA60B94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
   <si>
     <t>Sistem Informasi Penjualan</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>alamat dapat dimiliki banyak costumer</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>produk_id</t>
   </si>
 </sst>
 </file>
@@ -368,11 +374,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,30 +385,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,9 +410,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="135"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -434,6 +419,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EDBB8A-295C-4B0B-8A6D-A687DCBC7842}">
-  <dimension ref="D4:P78"/>
+  <dimension ref="C4:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="76" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="76" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,303 +759,305 @@
     <col min="6" max="6" width="20.453125" customWidth="1"/>
     <col min="7" max="7" width="18.26953125" customWidth="1"/>
     <col min="8" max="8" width="14.81640625" customWidth="1"/>
-    <col min="9" max="9" width="23.1796875" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
     <col min="12" max="12" width="16.81640625" customWidth="1"/>
     <col min="13" max="13" width="18.90625" customWidth="1"/>
     <col min="14" max="14" width="17.90625" customWidth="1"/>
     <col min="15" max="15" width="17.453125" customWidth="1"/>
+    <col min="16" max="16" width="9.54296875" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="6" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17">
         <v>45200</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>101</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="6">
-        <v>2</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="K7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
         <v>6000000</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="12">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3">
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="2">
         <v>102</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="6">
-        <v>3</v>
-      </c>
-      <c r="M8" s="3">
+      <c r="K8" s="16"/>
+      <c r="L8" s="4">
+        <v>3</v>
+      </c>
+      <c r="M8" s="2">
         <v>2000000</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="12">
         <v>0.08</v>
       </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3">
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="2">
         <v>103</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="6">
-        <v>3</v>
-      </c>
-      <c r="M9" s="3">
+      <c r="K9" s="16"/>
+      <c r="L9" s="4">
+        <v>3</v>
+      </c>
+      <c r="M9" s="2">
         <v>3000000</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="12">
         <v>0.06</v>
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="16">
+        <v>2</v>
+      </c>
+      <c r="E10" s="17">
         <v>45505</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>104</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="6">
+      <c r="K10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4">
         <v>5</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="16">
         <v>20000</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="12">
         <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3">
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="2">
         <v>105</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6">
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="4">
         <v>5</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="18">
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="D12" s="16">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17">
         <v>45233</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>106</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="4">
         <v>6</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="2">
         <v>6000</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.35">
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3">
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="2">
         <v>107</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="6">
+      <c r="K13" s="16"/>
+      <c r="L13" s="4">
         <v>7</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="2">
         <v>9000</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="13">
         <v>0.03</v>
       </c>
     </row>
@@ -1067,306 +1067,306 @@
       </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="10" t="s">
+      <c r="J18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="M18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="O18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D19" s="13">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
         <v>45200</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>101</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="6">
-        <v>2</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="2">
         <v>6000000</v>
       </c>
-      <c r="N19" s="7" t="s">
+      <c r="N19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19" s="12">
         <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D20" s="13">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9">
         <v>45201</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>102</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="6">
-        <v>3</v>
-      </c>
-      <c r="M20" s="3">
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="4">
+        <v>3</v>
+      </c>
+      <c r="M20" s="2">
         <v>2000000</v>
       </c>
-      <c r="N20" s="7" t="s">
+      <c r="N20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="12">
         <v>0.08</v>
       </c>
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D21" s="13">
-        <v>1</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9">
         <v>45202</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>103</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="6">
-        <v>3</v>
-      </c>
-      <c r="M21" s="3">
+      <c r="K21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="4">
+        <v>3</v>
+      </c>
+      <c r="M21" s="2">
         <v>3000000</v>
       </c>
-      <c r="N21" s="7" t="s">
+      <c r="N21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="12">
         <v>0.06</v>
       </c>
     </row>
     <row r="22" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D22" s="14">
-        <v>2</v>
-      </c>
-      <c r="E22" s="16">
+      <c r="D22" s="8">
+        <v>2</v>
+      </c>
+      <c r="E22" s="10">
         <v>45505</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>104</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="K22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L22" s="4">
         <v>5</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="3">
         <v>20000</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="N22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="12">
         <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D23" s="14">
-        <v>2</v>
-      </c>
-      <c r="E23" s="16">
+      <c r="D23" s="8">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10">
         <v>45506</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>105</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="K23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="4">
         <v>5</v>
       </c>
-      <c r="M23" s="13">
+      <c r="M23" s="3">
         <v>20000</v>
       </c>
-      <c r="N23" s="17" t="s">
+      <c r="N23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O23" s="18">
+      <c r="O23" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D24" s="13">
-        <v>3</v>
-      </c>
-      <c r="E24" s="16">
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10">
         <v>45233</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>106</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="4">
         <v>6</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="2">
         <v>6000</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D25" s="13">
-        <v>3</v>
-      </c>
-      <c r="E25" s="16">
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="E25" s="10">
         <v>45234</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>107</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="4">
         <v>7</v>
       </c>
-      <c r="M25" s="8">
+      <c r="M25" s="2">
         <v>9000</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O25" s="20">
+      <c r="O25" s="13">
         <v>0.03</v>
       </c>
     </row>
@@ -1381,282 +1381,282 @@
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J32" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M32" s="10" t="s">
+      <c r="M32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N32" s="10" t="s">
+      <c r="N32" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="15">
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
         <v>45200</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>101</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="6">
-        <v>2</v>
-      </c>
-      <c r="L33" s="3">
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2</v>
+      </c>
+      <c r="L33" s="2">
         <v>6000000</v>
       </c>
-      <c r="M33" s="7" t="s">
+      <c r="M33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N33" s="18">
+      <c r="N33" s="12">
         <v>0.1</v>
       </c>
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D34" s="13">
-        <v>1</v>
-      </c>
-      <c r="E34" s="15">
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="9">
         <v>45201</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>102</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J34" s="3">
-        <v>2</v>
-      </c>
-      <c r="K34" s="6">
-        <v>3</v>
-      </c>
-      <c r="L34" s="3">
+      <c r="J34" s="2">
+        <v>2</v>
+      </c>
+      <c r="K34" s="4">
+        <v>3</v>
+      </c>
+      <c r="L34" s="2">
         <v>2000000</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="M34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N34" s="18">
+      <c r="N34" s="12">
         <v>0.08</v>
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="15">
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
         <v>45202</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>103</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="3">
-        <v>3</v>
-      </c>
-      <c r="K35" s="6">
-        <v>3</v>
-      </c>
-      <c r="L35" s="3">
+      <c r="J35" s="2">
+        <v>3</v>
+      </c>
+      <c r="K35" s="4">
+        <v>3</v>
+      </c>
+      <c r="L35" s="2">
         <v>3000000</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="18">
+      <c r="N35" s="12">
         <v>0.06</v>
       </c>
     </row>
     <row r="36" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D36" s="14">
-        <v>2</v>
-      </c>
-      <c r="E36" s="16">
+      <c r="D36" s="8">
+        <v>2</v>
+      </c>
+      <c r="E36" s="10">
         <v>45505</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>104</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <v>4</v>
       </c>
-      <c r="K36" s="6">
+      <c r="K36" s="4">
         <v>5</v>
       </c>
-      <c r="L36" s="13">
+      <c r="L36" s="3">
         <v>20000</v>
       </c>
-      <c r="M36" s="17" t="s">
+      <c r="M36" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N36" s="18">
+      <c r="N36" s="12">
         <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D37" s="14">
-        <v>2</v>
-      </c>
-      <c r="E37" s="16">
+      <c r="D37" s="8">
+        <v>2</v>
+      </c>
+      <c r="E37" s="10">
         <v>45506</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>105</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="2">
         <v>5</v>
       </c>
-      <c r="K37" s="6">
+      <c r="K37" s="4">
         <v>5</v>
       </c>
-      <c r="L37" s="13">
+      <c r="L37" s="3">
         <v>20000</v>
       </c>
-      <c r="M37" s="17" t="s">
+      <c r="M37" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N37" s="18">
+      <c r="N37" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="38" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D38" s="13">
-        <v>3</v>
-      </c>
-      <c r="E38" s="16">
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="10">
         <v>45233</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>106</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="I38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="2">
         <v>6</v>
       </c>
-      <c r="K38" s="6">
+      <c r="K38" s="4">
         <v>6</v>
       </c>
-      <c r="L38" s="8">
+      <c r="L38" s="2">
         <v>6000</v>
       </c>
-      <c r="M38" s="9" t="s">
+      <c r="M38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N38" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D39" s="13">
-        <v>3</v>
-      </c>
-      <c r="E39" s="16">
+      <c r="D39" s="3">
+        <v>3</v>
+      </c>
+      <c r="E39" s="10">
         <v>45234</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>107</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="2">
         <v>7</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K39" s="4">
         <v>7</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L39" s="2">
         <v>9000</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="M39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N39" s="20">
+      <c r="N39" s="13">
         <v>0.03</v>
       </c>
     </row>
@@ -1666,30 +1666,30 @@
       </c>
     </row>
     <row r="43" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D44" s="3">
-        <v>1</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G44" s="3">
+      <c r="F44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="2">
         <v>6000000</v>
       </c>
       <c r="I44" t="s">
@@ -1697,16 +1697,16 @@
       </c>
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D45" s="3">
-        <v>2</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="D45" s="2">
+        <v>2</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F45" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G45" s="3">
+      <c r="F45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="2">
         <v>2000000</v>
       </c>
       <c r="I45" t="s">
@@ -1714,16 +1714,16 @@
       </c>
     </row>
     <row r="46" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D46" s="3">
-        <v>3</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="2">
+        <v>3</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F46" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G46" s="3">
+      <c r="F46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G46" s="2">
         <v>3000000</v>
       </c>
       <c r="I46" t="s">
@@ -1731,16 +1731,16 @@
       </c>
     </row>
     <row r="47" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>4</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="13">
+      <c r="F47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="3">
         <v>20000</v>
       </c>
       <c r="I47" t="s">
@@ -1748,16 +1748,16 @@
       </c>
     </row>
     <row r="48" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>5</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="13">
+      <c r="F48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="3">
         <v>20000</v>
       </c>
       <c r="I48" t="s">
@@ -1765,16 +1765,16 @@
       </c>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>6</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="2">
         <v>6000</v>
       </c>
       <c r="I49" t="s">
@@ -1782,16 +1782,16 @@
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>7</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F50" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="2">
         <v>9000</v>
       </c>
     </row>
@@ -1817,206 +1817,182 @@
       </c>
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E56" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="10" t="s">
+      <c r="E56" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="G56" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="H56" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="J56" t="s">
         <v>58</v>
       </c>
-      <c r="M56" s="21" t="s">
+      <c r="M56" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="N56" s="10" t="s">
+      <c r="N56" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D57" s="3">
-        <v>1</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="13">
-        <v>1</v>
-      </c>
-      <c r="G57" s="3">
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2">
         <v>6000000</v>
       </c>
-      <c r="H57" s="3">
-        <v>101</v>
-      </c>
-      <c r="J57" s="21" t="s">
+      <c r="J57" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K57" s="10" t="s">
+      <c r="K57" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M57" s="14"/>
-      <c r="N57" s="6"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="4"/>
     </row>
     <row r="58" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D58" s="3">
-        <v>2</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F58" s="13">
-        <v>1</v>
-      </c>
-      <c r="G58" s="3">
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2">
         <v>2000000</v>
       </c>
-      <c r="H58" s="3">
-        <v>102</v>
-      </c>
-      <c r="J58" s="14"/>
-      <c r="K58" s="6"/>
-      <c r="M58" s="3">
-        <v>1</v>
-      </c>
-      <c r="N58" s="3" t="s">
+      <c r="J58" s="8"/>
+      <c r="K58" s="4"/>
+      <c r="M58" s="2">
+        <v>1</v>
+      </c>
+      <c r="N58" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="59" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D59" s="3">
-        <v>3</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="2">
+        <v>3</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="13">
-        <v>1</v>
-      </c>
-      <c r="G59" s="3">
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="2">
         <v>3000000</v>
       </c>
-      <c r="H59" s="3">
-        <v>103</v>
-      </c>
-      <c r="J59" s="3">
-        <v>1</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M59" s="3">
-        <v>2</v>
-      </c>
-      <c r="N59" s="3" t="s">
+      <c r="J59" s="2">
+        <v>1</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M59" s="2">
+        <v>2</v>
+      </c>
+      <c r="N59" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="60" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>4</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E60" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="13">
-        <v>2</v>
-      </c>
-      <c r="G60" s="13">
+      <c r="F60" s="3">
+        <v>2</v>
+      </c>
+      <c r="G60" s="3">
         <v>20000</v>
       </c>
-      <c r="H60" s="3">
-        <v>104</v>
-      </c>
-      <c r="J60" s="3">
-        <v>2</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M60" s="3">
-        <v>3</v>
-      </c>
-      <c r="N60" s="3" t="s">
+      <c r="J60" s="2">
+        <v>2</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M60" s="2">
+        <v>3</v>
+      </c>
+      <c r="N60" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D61" s="3">
+      <c r="D61" s="2">
         <v>5</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="13">
-        <v>2</v>
-      </c>
-      <c r="G61" s="13">
+      <c r="F61" s="3">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3">
         <v>20000</v>
       </c>
-      <c r="H61" s="3">
-        <v>105</v>
-      </c>
-      <c r="J61" s="3">
-        <v>3</v>
-      </c>
-      <c r="K61" s="3" t="s">
+      <c r="J61" s="2">
+        <v>3</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M61" s="3">
+      <c r="M61" s="2">
         <v>4</v>
       </c>
-      <c r="N61" s="3" t="s">
+      <c r="N61" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="62" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D62" s="3">
+      <c r="D62" s="2">
         <v>6</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="13">
-        <v>3</v>
-      </c>
-      <c r="G62" s="8">
+      <c r="F62" s="3">
+        <v>3</v>
+      </c>
+      <c r="G62" s="2">
         <v>6000</v>
       </c>
-      <c r="H62" s="3">
-        <v>106</v>
-      </c>
-      <c r="M62" s="3">
+      <c r="M62" s="2">
         <v>5</v>
       </c>
-      <c r="N62" s="3" t="s">
+      <c r="N62" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="63" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <v>7</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F63" s="13">
-        <v>3</v>
-      </c>
-      <c r="G63" s="8">
+      <c r="F63" s="3">
+        <v>3</v>
+      </c>
+      <c r="G63" s="2">
         <v>9000</v>
-      </c>
-      <c r="H63" s="3">
-        <v>107</v>
       </c>
       <c r="I63" t="s">
         <v>67</v>
@@ -2030,264 +2006,337 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:18" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
         <v>57</v>
       </c>
-      <c r="J65" t="s">
-        <v>60</v>
-      </c>
       <c r="O65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D66" s="10" t="s">
+      <c r="R65" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C66" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="10" t="s">
+      <c r="F66" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G66" s="10" t="s">
+      <c r="G66" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="10" t="s">
+      <c r="H66" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J66" s="10" t="s">
+      <c r="I66" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
+        <v>101</v>
+      </c>
+      <c r="E67" s="3">
+        <v>1</v>
+      </c>
+      <c r="F67" s="9">
+        <v>45200</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I67" s="4">
+        <v>1</v>
+      </c>
+      <c r="K67" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K66" s="10" t="s">
+      <c r="L67" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L66" s="10" t="s">
+      <c r="M67" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M66" s="10" t="s">
+      <c r="N67" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O66" s="22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D67" s="3">
+      <c r="O67" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C68" s="4">
+        <v>2</v>
+      </c>
+      <c r="D68" s="2">
+        <v>102</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+      <c r="F68" s="9">
+        <v>45201</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="I68" s="4">
+        <v>2</v>
+      </c>
+      <c r="K68" s="2">
         <v>101</v>
       </c>
-      <c r="E67" s="13">
-        <v>1</v>
-      </c>
-      <c r="F67" s="15">
-        <v>45200</v>
-      </c>
-      <c r="G67" s="7" t="s">
+      <c r="L68" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M68" s="2">
+        <v>1</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C69" s="4">
+        <v>3</v>
+      </c>
+      <c r="D69" s="2">
+        <v>103</v>
+      </c>
+      <c r="E69" s="3">
+        <v>1</v>
+      </c>
+      <c r="F69" s="9">
+        <v>45202</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H67" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="J67" s="3">
-        <v>101</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L67" s="3">
-        <v>1</v>
-      </c>
-      <c r="M67" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D68" s="3">
+      <c r="H69" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="I69" s="4">
+        <v>3</v>
+      </c>
+      <c r="K69" s="2">
         <v>102</v>
       </c>
-      <c r="E68" s="13">
-        <v>1</v>
-      </c>
-      <c r="F68" s="15">
-        <v>45201</v>
-      </c>
-      <c r="G68" s="7" t="s">
+      <c r="L69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M69" s="2">
+        <v>1</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O69" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C70" s="4">
+        <v>4</v>
+      </c>
+      <c r="D70" s="2">
+        <v>104</v>
+      </c>
+      <c r="E70" s="8">
+        <v>2</v>
+      </c>
+      <c r="F70" s="10">
+        <v>45505</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H70" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="I70" s="4">
+        <v>4</v>
+      </c>
+      <c r="K70" s="2">
+        <v>103</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M70" s="2">
+        <v>4</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O70" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C71" s="4">
+        <v>5</v>
+      </c>
+      <c r="D71" s="2">
+        <v>105</v>
+      </c>
+      <c r="E71" s="8">
+        <v>2</v>
+      </c>
+      <c r="F71" s="10">
+        <v>45506</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H71" s="12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I71" s="4">
+        <v>5</v>
+      </c>
+      <c r="K71" s="2">
+        <v>104</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M71" s="2">
+        <v>2</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O71" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C72" s="4">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2">
+        <v>106</v>
+      </c>
+      <c r="E72" s="3">
+        <v>3</v>
+      </c>
+      <c r="F72" s="10">
+        <v>45233</v>
+      </c>
+      <c r="G72" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H68" s="18">
-        <v>0.08</v>
-      </c>
-      <c r="J68" s="3">
-        <v>102</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L68" s="3">
-        <v>1</v>
-      </c>
-      <c r="M68" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D69" s="3">
-        <v>103</v>
-      </c>
-      <c r="E69" s="13">
-        <v>1</v>
-      </c>
-      <c r="F69" s="15">
-        <v>45202</v>
-      </c>
-      <c r="G69" s="7" t="s">
+      <c r="H72" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="I72" s="4">
+        <v>6</v>
+      </c>
+      <c r="K72" s="2">
+        <v>105</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M72" s="2">
+        <v>3</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O72" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C73" s="4">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2">
+        <v>107</v>
+      </c>
+      <c r="E73" s="3">
+        <v>3</v>
+      </c>
+      <c r="F73" s="10">
+        <v>45234</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H69" s="18">
-        <v>0.06</v>
-      </c>
-      <c r="J69" s="3">
-        <v>103</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L69" s="3">
-        <v>4</v>
-      </c>
-      <c r="M69" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D70" s="3">
-        <v>104</v>
-      </c>
-      <c r="E70" s="14">
-        <v>2</v>
-      </c>
-      <c r="F70" s="16">
-        <v>45505</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="H70" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="J70" s="3">
-        <v>104</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L70" s="3">
-        <v>2</v>
-      </c>
-      <c r="M70" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="71" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D71" s="3">
-        <v>105</v>
-      </c>
-      <c r="E71" s="14">
-        <v>2</v>
-      </c>
-      <c r="F71" s="16">
-        <v>45506</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="H71" s="18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J71" s="3">
-        <v>105</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L71" s="3">
-        <v>3</v>
-      </c>
-      <c r="M71" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D72" s="3">
+      <c r="H73" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="I73" s="4">
+        <v>7</v>
+      </c>
+      <c r="K73" s="2">
         <v>106</v>
       </c>
-      <c r="E72" s="13">
-        <v>3</v>
-      </c>
-      <c r="F72" s="16">
-        <v>45233</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H72" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="J72" s="3">
-        <v>106</v>
-      </c>
-      <c r="K72" s="3" t="s">
+      <c r="L73" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L72" s="3">
-        <v>1</v>
-      </c>
-      <c r="M72" s="6" t="s">
+      <c r="M73" s="2">
+        <v>1</v>
+      </c>
+      <c r="N73" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="73" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D73" s="3">
+      <c r="O73" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="K74" s="2">
         <v>107</v>
       </c>
-      <c r="E73" s="13">
-        <v>3</v>
-      </c>
-      <c r="F73" s="16">
-        <v>45234</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H73" s="20">
-        <v>0.03</v>
-      </c>
-      <c r="J73" s="3">
-        <v>107</v>
-      </c>
-      <c r="K73" s="3" t="s">
+      <c r="L74" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L73" s="3">
+      <c r="M74" s="2">
         <v>5</v>
       </c>
-      <c r="M73" s="6" t="s">
+      <c r="N74" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O73" s="19"/>
-    </row>
-    <row r="76" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="O74" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="3:18" x14ac:dyDescent="0.35">
       <c r="I76" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:18" x14ac:dyDescent="0.35">
       <c r="I77" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:18" x14ac:dyDescent="0.35">
       <c r="I78" t="s">
         <v>63</v>
       </c>
@@ -2298,11 +2347,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="13">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="D4:O4"/>
     <mergeCell ref="K7:K9"/>
@@ -2311,6 +2355,11 @@
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="N10:N11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>